<commit_message>
(Planilha gerada com vendas atualizadas)
</commit_message>
<xml_diff>
--- a/relatorio_vendas.xlsx
+++ b/relatorio_vendas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,242 +440,974 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id_venda</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>data_venda</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>quantidade</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_cliente</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cliente</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>cidade</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>id_produto</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>produto</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>categoria</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>cliente</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>cidade</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>preco</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>quantidade</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>total</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>mes</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>45301</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Notebook</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Eletrônicos</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
-      </c>
-      <c r="F2" t="n">
-        <v>3000</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Notebook</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>3000</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>2024-01</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>45301</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Eletrônicos</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>São Paulo</t>
         </is>
-      </c>
-      <c r="F3" t="n">
-        <v>50</v>
       </c>
       <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>50</v>
+      </c>
+      <c r="K3" t="n">
         <v>100</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>2024-01</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>45327</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bruno</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Caderno</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Papelaria</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="J4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K4" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2024-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>45332</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Carla</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Curitiba</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Caneta</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Papelaria</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2024-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>45352</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Bruno</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Rio de Janeiro</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Notebook</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3000</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2024-03</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>45413</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Notebook</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="K7" t="n">
+        <v>6000</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>45414</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bruno</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>50</v>
+      </c>
+      <c r="K8" t="n">
+        <v>50</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>45415</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Carla</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Curitiba</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Caderno</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Papelaria</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
         <v>20</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K9" t="n">
+        <v>80</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>45416</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Carlos Silva</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Caneta</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Papelaria</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
         <v>5</v>
       </c>
-      <c r="H4" t="n">
-        <v>100</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2024-02</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45352</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Notebook</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="K10" t="n">
+        <v>5</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>45417</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Smartphone Samsung Galaxy S22</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>Eletrônicos</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="J11" t="n">
+        <v>4299.9</v>
+      </c>
+      <c r="K11" t="n">
+        <v>12899.7</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>45418</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Marcos Lima</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Belo Horizonte</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Notebook Dell Inspiron 15</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>3899</v>
+      </c>
+      <c r="K12" t="n">
+        <v>7798</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>45419</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Fernanda Oliveira</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Curitiba</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>7</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Smart TV LG 55" 4K</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>2999.9</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2999.9</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>45420</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Rafael Costa</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Porto Alegre</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>8</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Fone de Ouvido JBL Bluetooth</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>399.9</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1999.5</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>45421</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>9</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>PlayStation 5</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>4499.9</v>
+      </c>
+      <c r="K15" t="n">
+        <v>8999.799999999999</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Bruno</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Rio de Janeiro</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>3000</v>
-      </c>
-      <c r="G5" t="n">
+      <c r="G16" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Mouse Gamer Logitech G502</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>299.9</v>
+      </c>
+      <c r="K16" t="n">
+        <v>299.9</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>45423</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Carla</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Curitiba</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>11</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Teclado Mecânico Redragon</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>349.9</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1049.7</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>45424</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Carlos Silva</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>12</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Monitor Samsung 24" LED</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>799.9</v>
+      </c>
+      <c r="K18" t="n">
+        <v>1599.8</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>45425</v>
+      </c>
+      <c r="C19" t="n">
         <v>1</v>
       </c>
-      <c r="H5" t="n">
-        <v>3000</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2024-03</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45332</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Caneta</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Papelaria</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Carla</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Curitiba</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
+      <c r="D19" t="n">
         <v>5</v>
       </c>
-      <c r="G6" t="n">
-        <v>10</v>
-      </c>
-      <c r="H6" t="n">
-        <v>50</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2024-02</t>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Ana Souza</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>13</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Caixa de Som Bluetooth JBL Flip 6</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>599.9</v>
+      </c>
+      <c r="K19" t="n">
+        <v>599.9</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2024-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>45426</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Marcos Lima</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Belo Horizonte</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>14</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Echo Dot (Alexa) 5ª Geração</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Eletrônicos</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>349</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1396</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2024-05</t>
         </is>
       </c>
     </row>

</xml_diff>